<commit_message>
add notification for wrong raw occurrence dataset
</commit_message>
<xml_diff>
--- a/Data/ex3.Lead (Pb)-2016_2017 with ProcessFacets.xlsx
+++ b/Data/ex3.Lead (Pb)-2016_2017 with ProcessFacets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\IMPROVAST\SGL\foodex2.shiny\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37AC5B6A-E284-4FF5-82D8-5E650834E4E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4990F06E-7A90-4411-B6C5-C0FFE531FFF6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29610" yWindow="-120" windowWidth="28110" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -204,7 +204,7 @@
     <t>Potatoes  {Mixing}</t>
   </si>
   <si>
-    <t>A00ZT#F28.A0CRl</t>
+    <t>A00ZT#F28.A0CRlss</t>
   </si>
 </sst>
 </file>
@@ -212,7 +212,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -297,7 +297,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -311,11 +311,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -657,7 +657,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="E23" sqref="E23:J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1334,28 +1334,28 @@
         <v>8</v>
       </c>
       <c r="E21" s="8">
-        <f>E12*0.7</f>
-        <v>1.2343333333333331E-2</v>
+        <f>E12*2</f>
+        <v>3.5266666666666661E-2</v>
       </c>
       <c r="F21" s="8">
-        <f t="shared" ref="F21:J21" si="1">F12*0.7</f>
-        <v>8.3999999999999995E-3</v>
+        <f t="shared" ref="F21:J21" si="1">F12*2</f>
+        <v>2.4E-2</v>
       </c>
       <c r="G21" s="8">
         <f t="shared" si="1"/>
-        <v>1.2343333333333331E-2</v>
+        <v>3.5266666666666661E-2</v>
       </c>
       <c r="H21" s="8">
         <f t="shared" si="1"/>
-        <v>8.3999999999999995E-3</v>
+        <v>2.4E-2</v>
       </c>
       <c r="I21" s="8">
         <f t="shared" si="1"/>
-        <v>1.2343333333333331E-2</v>
+        <v>3.5266666666666661E-2</v>
       </c>
       <c r="J21" s="8">
         <f t="shared" si="1"/>
-        <v>8.3999999999999995E-3</v>
+        <v>2.4E-2</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1372,28 +1372,28 @@
         <v>8</v>
       </c>
       <c r="E22" s="8">
-        <f>E12*0.7</f>
-        <v>1.2343333333333331E-2</v>
+        <f>E12*2</f>
+        <v>3.5266666666666661E-2</v>
       </c>
       <c r="F22" s="8">
-        <f t="shared" ref="F22:J23" si="2">F12*0.7</f>
-        <v>8.3999999999999995E-3</v>
+        <f t="shared" ref="F22:J22" si="2">F12*2</f>
+        <v>2.4E-2</v>
       </c>
       <c r="G22" s="8">
         <f t="shared" si="2"/>
-        <v>1.2343333333333331E-2</v>
+        <v>3.5266666666666661E-2</v>
       </c>
       <c r="H22" s="8">
         <f t="shared" si="2"/>
-        <v>8.3999999999999995E-3</v>
+        <v>2.4E-2</v>
       </c>
       <c r="I22" s="8">
         <f t="shared" si="2"/>
-        <v>1.2343333333333331E-2</v>
+        <v>3.5266666666666661E-2</v>
       </c>
       <c r="J22" s="8">
         <f t="shared" si="2"/>
-        <v>8.3999999999999995E-3</v>
+        <v>2.4E-2</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1410,28 +1410,28 @@
         <v>8</v>
       </c>
       <c r="E23" s="12">
-        <f>E13*0.7</f>
-        <v>2.6162499999999997E-3</v>
+        <f>E13*2</f>
+        <v>7.4749999999999999E-3</v>
       </c>
       <c r="F23" s="12">
-        <f t="shared" si="2"/>
-        <v>1.4699999999999997E-3</v>
+        <f t="shared" ref="F23:J23" si="3">F13*2</f>
+        <v>4.1999999999999997E-3</v>
       </c>
       <c r="G23" s="12">
-        <f t="shared" si="2"/>
-        <v>3.05375E-3</v>
+        <f t="shared" si="3"/>
+        <v>8.7250000000000001E-3</v>
       </c>
       <c r="H23" s="12">
-        <f t="shared" si="2"/>
-        <v>1.9599999999999999E-3</v>
+        <f t="shared" si="3"/>
+        <v>5.5999999999999999E-3</v>
       </c>
       <c r="I23" s="12">
-        <f t="shared" si="2"/>
-        <v>3.4912499999999996E-3</v>
+        <f t="shared" si="3"/>
+        <v>9.9749999999999995E-3</v>
       </c>
       <c r="J23" s="12">
-        <f t="shared" si="2"/>
-        <v>2.4499999999999999E-3</v>
+        <f t="shared" si="3"/>
+        <v>7.0000000000000001E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>